<commit_message>
Domain and mesh converegence is done
</commit_message>
<xml_diff>
--- a/CFD files/Drag lift.xlsx
+++ b/CFD files/Drag lift.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoa-my.sharepoint.com/personal/mter153_uoa_auckland_ac_nz/Documents/Documents/ENGSCI 344/Assignment/Plane_wing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoa-my.sharepoint.com/personal/mter153_uoa_auckland_ac_nz/Documents/Documents/ENGSCI 344/Assignment/Plane_wing/CFD files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="11_F25DC773A252ABDACC1048D8295E7C125ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF9B0EDF-B06C-4B91-A634-58C7041A45A7}"/>
+  <xr:revisionPtr revIDLastSave="233" documentId="13_ncr:1_{6A96FC55-E235-4CFF-85EA-4344623012AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{140E732B-94D6-421E-9A22-5424D66066D3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>Domain area</t>
   </si>
@@ -60,13 +60,97 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here we can see clear convergence </t>
+  </si>
+  <si>
+    <t>Will use option highlighted as red for domain</t>
+  </si>
+  <si>
+    <t>Final Domain options</t>
+  </si>
+  <si>
+    <t>H6</t>
+  </si>
+  <si>
+    <t>H7</t>
+  </si>
+  <si>
+    <t>V8</t>
+  </si>
+  <si>
+    <t>V9</t>
+  </si>
+  <si>
+    <t>Mesh convergence</t>
+  </si>
+  <si>
+    <t>0.06 m</t>
+  </si>
+  <si>
+    <t>0.05 m</t>
+  </si>
+  <si>
+    <t>0.04 m</t>
+  </si>
+  <si>
+    <t>0.03 m</t>
+  </si>
+  <si>
+    <t>0.01 m</t>
+  </si>
+  <si>
+    <t>Mean mesh size</t>
+  </si>
+  <si>
+    <t>0.08 m</t>
+  </si>
+  <si>
+    <t>Node count</t>
+  </si>
+  <si>
+    <t>Mean mesh size difference</t>
+  </si>
+  <si>
+    <t>Choose this one</t>
+  </si>
+  <si>
+    <t>Too slow</t>
+  </si>
+  <si>
+    <t>Domain is far too big</t>
+  </si>
+  <si>
+    <t>Converged and little change between drag and lift coefficeints</t>
+  </si>
+  <si>
+    <t>Element size (fine mesh)</t>
+  </si>
+  <si>
+    <t>Element size (coarse mesh)</t>
+  </si>
+  <si>
+    <t>0.5 m</t>
+  </si>
+  <si>
+    <t>0.02 m</t>
+  </si>
+  <si>
+    <t>0.005 m</t>
+  </si>
+  <si>
+    <t>0.02 m fine mesh and 0.5 coarse mesh seems to be best option.</t>
+  </si>
+  <si>
+    <t>The mean mesh size criteria is satisfied and so this is good.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,8 +158,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -85,6 +183,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -101,9 +217,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,100 +506,642 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
     <col min="7" max="7" width="23.7109375" customWidth="1"/>
+    <col min="8" max="8" width="24" customWidth="1"/>
+    <col min="9" max="9" width="56.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2.0611999999999999</v>
+      </c>
+      <c r="B2">
+        <v>0.71845999999999999</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C10" si="0">A2*B2</f>
+        <v>1.4808897519999999</v>
+      </c>
       <c r="D2">
-        <v>100</v>
+        <v>2.9554008999999999E-2</v>
+      </c>
+      <c r="E2">
+        <v>0.71810739999999995</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3.6280000000000001</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>7.2560000000000002</v>
+      </c>
       <c r="D3">
-        <v>90</v>
+        <v>1.1324624E-2</v>
+      </c>
+      <c r="E3">
+        <v>0.34481457999999998</v>
       </c>
       <c r="F3">
-        <f>(D2-D3)/D2*100</f>
+        <f t="shared" ref="F3:G10" si="1">(D2-D3)/D2*100</f>
+        <v>61.681597917900078</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="1"/>
+        <v>51.982867743738616</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5.6280000000000001</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>22.512</v>
+      </c>
+      <c r="D4">
+        <v>1.0276176E-2</v>
+      </c>
+      <c r="E4">
+        <v>0.30429148</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>9.2581263625176469</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>11.752142267302032</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>5.8280000000000003</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
+        <v>24.477600000000002</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.0197199000000001E-2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.30180785999999998</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="1"/>
+        <v>0.7685446415086622</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="1"/>
+        <v>0.81619767993504777</v>
+      </c>
+      <c r="I5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>6.8280000000000003</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="0"/>
+        <v>35.505600000000001</v>
+      </c>
+      <c r="D6">
+        <v>1.0371132E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.2913675</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="1"/>
+        <v>-1.7056938871154657</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="1"/>
+        <v>3.4592737246803256</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>9.6280000000000001</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>77.024000000000001</v>
+      </c>
+      <c r="D7">
+        <v>9.8964685999999996E-3</v>
+      </c>
+      <c r="E7">
+        <v>0.29569980000000001</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="1"/>
+        <v>4.576775225693785</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="1"/>
+        <v>-1.4868851193080941</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="D8">
+        <v>9.8720054999999994E-3</v>
+      </c>
+      <c r="E8">
+        <v>0.29475685000000001</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.24719019469227854</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.31888760154724416</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>288</v>
+      </c>
+      <c r="D9">
+        <v>9.8491657000000007E-3</v>
+      </c>
+      <c r="E9">
+        <v>0.29136630000000002</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.23135927142664917</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1502870925645974</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>32</v>
+      </c>
+      <c r="B10">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>448</v>
+      </c>
+      <c r="D10">
+        <v>9.7028710000000001E-3</v>
+      </c>
+      <c r="E10">
+        <v>0.29177199999999998</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="1"/>
+        <v>1.4853511907105046</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.1392405367401629</v>
+      </c>
+      <c r="H10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D4">
-        <v>80</v>
-      </c>
-      <c r="F4">
-        <f t="shared" ref="F4:F7" si="0">(D3-D4)/D3*100</f>
-        <v>11.111111111111111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D5">
-        <v>77</v>
-      </c>
-      <c r="F5" s="1">
-        <f t="shared" si="0"/>
-        <v>3.75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D6">
-        <v>75</v>
-      </c>
-      <c r="F6" s="1">
-        <f t="shared" si="0"/>
-        <v>2.5974025974025974</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D7">
-        <v>73</v>
-      </c>
-      <c r="F7" s="1">
-        <f t="shared" si="0"/>
-        <v>2.666666666666667</v>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="1">
+        <v>10306</v>
+      </c>
+      <c r="D19" s="1">
+        <f>1/SQRT(C19)</f>
+        <v>9.8504241437690522E-3</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1.8544970000000001E-2</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.23978103000000001</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="1">
+        <v>14231</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" ref="D20:D26" si="2">1/SQRT(C20)</f>
+        <v>8.3826684755424017E-3</v>
+      </c>
+      <c r="E20" s="1">
+        <f>D19/D20</f>
+        <v>1.1750940851960245</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1.6968328000000001E-2</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.24687503</v>
+      </c>
+      <c r="H20">
+        <f>(F19-F20)/F19*100</f>
+        <v>8.501723108745928</v>
+      </c>
+      <c r="I20">
+        <f>(G19-G20)/G19*100</f>
+        <v>-2.9585326245366401</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21">
+        <v>17489</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="2"/>
+        <v>7.5616663574680359E-3</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" ref="E21:E26" si="3">D20/D21</f>
+        <v>1.1085742320888741</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1.5544442E-2</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.25375240999999998</v>
+      </c>
+      <c r="H21">
+        <f t="shared" ref="H21:H26" si="4">(F20-F21)/F20*100</f>
+        <v>8.3914337346614278</v>
+      </c>
+      <c r="I21">
+        <f t="shared" ref="I21:I26" si="5">(G20-G21)/G20*100</f>
+        <v>-2.7857738386907691</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22">
+        <v>23574</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="2"/>
+        <v>6.5130342260652473E-3</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="3"/>
+        <v>1.1610051621111017</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1.4040110999999999E-2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.26953092000000001</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="4"/>
+        <v>9.6776133874731638</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="5"/>
+        <v>-6.2180729633267422</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23">
+        <v>35299</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="2"/>
+        <v>5.322538344718966E-3</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="3"/>
+        <v>1.2236707007526764</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1.2465092000000001E-2</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.28641793999999998</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="4"/>
+        <v>11.217995356304511</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="5"/>
+        <v>-6.2653368303718082</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="7">
+        <v>93163</v>
+      </c>
+      <c r="D24" s="7">
+        <f t="shared" si="2"/>
+        <v>3.2762593054010284E-3</v>
+      </c>
+      <c r="E24" s="7">
+        <f t="shared" si="3"/>
+        <v>1.6245778641344337</v>
+      </c>
+      <c r="F24" s="7">
+        <v>1.0974332E-2</v>
+      </c>
+      <c r="G24" s="7">
+        <v>0.26555524000000003</v>
+      </c>
+      <c r="H24" s="7">
+        <f t="shared" si="4"/>
+        <v>11.95947851808876</v>
+      </c>
+      <c r="I24" s="7">
+        <f t="shared" si="5"/>
+        <v>7.2840060228070751</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25">
+        <v>226459</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="2"/>
+        <v>2.1013829654395653E-3</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="3"/>
+        <v>1.5590967278616459</v>
+      </c>
+      <c r="F25">
+        <v>9.6322362999999994E-3</v>
+      </c>
+      <c r="G25">
+        <v>0.26390879</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="4"/>
+        <v>12.229406764803548</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="5"/>
+        <v>0.62000282878998036</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26">
+        <v>845227</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="2"/>
+        <v>1.0877104954927549E-3</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="3"/>
+        <v>1.9319322321033561</v>
+      </c>
+      <c r="F26">
+        <v>9.2090122999999996E-3</v>
+      </c>
+      <c r="G26">
+        <v>0.26414621999999999</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="4"/>
+        <v>4.3938290841141407</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="5"/>
+        <v>-8.9966688870038378E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>